<commit_message>
Moving stored procs here Organizing into folders
</commit_message>
<xml_diff>
--- a/CI/TestSQL/02.TestData/CreateEvent.xlsx
+++ b/CI/TestSQL/02.TestData/CreateEvent.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22485" windowHeight="7433"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22485" windowHeight="7433" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateEvent" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -971,874 +971,874 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.9296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1328125" customWidth="1"/>
-    <col min="12" max="12" width="47.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="47.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1">
+        <v>43101</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43459</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1">
-        <v>43101</v>
-      </c>
-      <c r="F2" s="1">
-        <v>43459</v>
-      </c>
-      <c r="G2">
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1">
+        <v>43459</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43465</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1">
-        <v>43459</v>
-      </c>
-      <c r="F3" s="1">
-        <v>43465</v>
-      </c>
-      <c r="G3">
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>14</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2">
+        <v>43091.416666666664</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43091.458333333336</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2">
-        <v>43091.416666666664</v>
-      </c>
-      <c r="F4" s="2">
-        <v>43091.458333333336</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
         <v>19</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2">
+        <v>43092.416666666664</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43092.458333333336</v>
+      </c>
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2">
-        <v>43092.416666666664</v>
-      </c>
-      <c r="F5" s="2">
-        <v>43092.458333333336</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2">
+        <v>43093.416666666664</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43093.458333333336</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2">
-        <v>43093.416666666664</v>
-      </c>
-      <c r="F6" s="2">
-        <v>43093.458333333336</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
         <v>19</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2">
+        <v>43094.416666666664</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43094.458333333336</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2">
-        <v>43094.416666666664</v>
-      </c>
-      <c r="F7" s="2">
-        <v>43094.458333333336</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
         <v>19</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2">
+        <v>43095.416666666664</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43095.458333333336</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="2">
-        <v>43095.416666666664</v>
-      </c>
-      <c r="F8" s="2">
-        <v>43095.458333333336</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2">
+        <v>43096.416666666664</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43096.458333333336</v>
+      </c>
+      <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2">
-        <v>43096.416666666664</v>
-      </c>
-      <c r="F9" s="2">
-        <v>43096.458333333336</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2">
+        <v>43091.625</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43091.666666666664</v>
+      </c>
+      <c r="D10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="2">
-        <v>43091.625</v>
-      </c>
-      <c r="F10" s="2">
-        <v>43091.666666666664</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2">
+        <v>43092.625</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43092.666666666664</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="2">
-        <v>43092.625</v>
-      </c>
-      <c r="F11" s="2">
-        <v>43092.666666666664</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="K11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2">
+        <v>43093.625</v>
+      </c>
+      <c r="C12" s="2">
+        <v>43093.666666666664</v>
+      </c>
+      <c r="D12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="2">
-        <v>43093.625</v>
-      </c>
-      <c r="F12" s="2">
-        <v>43093.666666666664</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>3</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+      <c r="K12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2">
+        <v>43094.625</v>
+      </c>
+      <c r="C13" s="2">
+        <v>43094.666666666664</v>
+      </c>
+      <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="2">
-        <v>43094.625</v>
-      </c>
-      <c r="F13" s="2">
-        <v>43094.666666666664</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>3</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2">
+        <v>43095.625</v>
+      </c>
+      <c r="C14" s="2">
+        <v>43095.666666666664</v>
+      </c>
+      <c r="D14" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="2">
-        <v>43095.625</v>
-      </c>
-      <c r="F14" s="2">
-        <v>43095.666666666664</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>3</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2">
+        <v>43096.625</v>
+      </c>
+      <c r="C15" s="2">
+        <v>43096.666666666664</v>
+      </c>
+      <c r="D15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="2">
-        <v>43096.625</v>
-      </c>
-      <c r="F15" s="2">
-        <v>43096.666666666664</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2">
+        <v>43091.458333333336</v>
+      </c>
+      <c r="C16" s="2">
+        <v>43091.5</v>
+      </c>
+      <c r="D16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="2">
-        <v>43091.458333333336</v>
-      </c>
-      <c r="F16" s="2">
-        <v>43091.5</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2">
+        <v>43098.458333333336</v>
+      </c>
+      <c r="C17" s="2">
+        <v>43098.5</v>
+      </c>
+      <c r="D17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="2">
-        <v>43098.458333333336</v>
-      </c>
-      <c r="F17" s="2">
-        <v>43098.5</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>3</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2">
+        <v>43105.458333333336</v>
+      </c>
+      <c r="C18" s="2">
+        <v>43105.5</v>
+      </c>
+      <c r="D18" t="s">
         <v>26</v>
       </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="2">
-        <v>43105.458333333336</v>
-      </c>
-      <c r="F18" s="2">
-        <v>43105.5</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>3</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2">
+        <v>43112.458333333336</v>
+      </c>
+      <c r="C19" s="2">
+        <v>43112.5</v>
+      </c>
+      <c r="D19" t="s">
         <v>26</v>
       </c>
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="2">
-        <v>43112.458333333336</v>
-      </c>
-      <c r="F19" s="2">
-        <v>43112.5</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>3</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2">
+        <v>43119.458333333336</v>
+      </c>
+      <c r="C20" s="2">
+        <v>43119.5</v>
+      </c>
+      <c r="D20" t="s">
         <v>26</v>
       </c>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="2">
-        <v>43119.458333333336</v>
-      </c>
-      <c r="F20" s="2">
-        <v>43119.5</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>3</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2">
+        <v>43126.458333333336</v>
+      </c>
+      <c r="C21" s="2">
+        <v>43126.5</v>
+      </c>
+      <c r="D21" t="s">
         <v>26</v>
       </c>
-      <c r="C21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="2">
-        <v>43126.458333333336</v>
-      </c>
-      <c r="F21" s="2">
-        <v>43126.5</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>3</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>28</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2">
+        <v>43091.541666666664</v>
+      </c>
+      <c r="C22" s="2">
+        <v>43091.625</v>
+      </c>
+      <c r="D22" t="s">
         <v>29</v>
       </c>
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="2">
-        <v>43091.541666666664</v>
-      </c>
-      <c r="F22" s="2">
-        <v>43091.625</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>3</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>28</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2">
+        <v>43098.541666666664</v>
+      </c>
+      <c r="C23" s="2">
+        <v>43098.625</v>
+      </c>
+      <c r="D23" t="s">
         <v>29</v>
       </c>
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="2">
-        <v>43098.541666666664</v>
-      </c>
-      <c r="F23" s="2">
-        <v>43098.625</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>3</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="K23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2">
+        <v>43105.541666666664</v>
+      </c>
+      <c r="C24" s="2">
+        <v>43105.625</v>
+      </c>
+      <c r="D24" t="s">
         <v>29</v>
       </c>
-      <c r="C24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="2">
-        <v>43105.541666666664</v>
-      </c>
-      <c r="F24" s="2">
-        <v>43105.625</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>3</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2">
+        <v>43112.541666666664</v>
+      </c>
+      <c r="C25" s="2">
+        <v>43112.625</v>
+      </c>
+      <c r="D25" t="s">
         <v>29</v>
       </c>
-      <c r="C25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="2">
-        <v>43112.541666666664</v>
-      </c>
-      <c r="F25" s="2">
-        <v>43112.625</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>3</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+      <c r="K25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2">
+        <v>43119.541666666664</v>
+      </c>
+      <c r="C26" s="2">
+        <v>43119.625</v>
+      </c>
+      <c r="D26" t="s">
         <v>29</v>
       </c>
-      <c r="C26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="2">
-        <v>43119.541666666664</v>
-      </c>
-      <c r="F26" s="2">
-        <v>43119.625</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="H26">
-        <v>3</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="E26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
+      <c r="K26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2">
+        <v>43126.541666666664</v>
+      </c>
+      <c r="C27" s="2">
+        <v>43126.625</v>
+      </c>
+      <c r="D27" t="s">
         <v>29</v>
       </c>
-      <c r="C27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="2">
-        <v>43126.541666666664</v>
-      </c>
-      <c r="F27" s="2">
-        <v>43126.625</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>3</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>3</v>
+      </c>
+      <c r="K27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2">
+        <v>43105.541666666664</v>
+      </c>
+      <c r="C28" s="2">
+        <v>43108.541666666664</v>
+      </c>
+      <c r="D28" t="s">
         <v>31</v>
       </c>
-      <c r="C28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="2">
-        <v>43105.541666666664</v>
-      </c>
-      <c r="F28" s="2">
-        <v>43108.541666666664</v>
-      </c>
-      <c r="G28">
+      <c r="I28">
         <v>6</v>
       </c>
-      <c r="H28">
+      <c r="J28">
         <v>5</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>34</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2">
+        <v>43105.541666666664</v>
+      </c>
+      <c r="C29" s="2">
+        <v>43108.541666666664</v>
+      </c>
+      <c r="D29" t="s">
         <v>35</v>
       </c>
-      <c r="C29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="2">
-        <v>43105.541666666664</v>
-      </c>
-      <c r="F29" s="2">
-        <v>43108.541666666664</v>
-      </c>
-      <c r="G29">
+      <c r="I29">
         <v>6</v>
       </c>
-      <c r="H29">
+      <c r="J29">
         <v>5</v>
       </c>
-      <c r="I29" t="s">
+      <c r="K29" t="s">
         <v>33</v>
       </c>
-      <c r="K29" t="s">
+      <c r="M29" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>